<commit_message>
Sports Scheduling and Selecting Hotels
Sports Scheduling and Selecting Hotels
</commit_message>
<xml_diff>
--- a/9IntegerProgramming/SelectingHotels.xlsx
+++ b/9IntegerProgramming/SelectingHotels.xlsx
@@ -1,15 +1,57 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3700" yWindow="300" windowWidth="19480" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="3705" yWindow="300" windowWidth="19485" windowHeight="11760" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Regression" sheetId="1" r:id="rId1"/>
+    <sheet name="Optimization" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">Optimization!$F$3:$F$18</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">Optimization!$D$22</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">Optimization!$D$23</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">Optimization!$D$24</definedName>
+    <definedName name="solver_lhs4" localSheetId="1" hidden="1">Optimization!$F$3:$F$18</definedName>
+    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">4</definedName>
+    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">Optimization!$D$24</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rel3" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="1" hidden="1">5</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">Optimization!$F$22</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">Optimization!$F$23</definedName>
+    <definedName name="solver_rhs3" localSheetId="1" hidden="1">Optimization!$F$24</definedName>
+    <definedName name="solver_rhs4" localSheetId="1" hidden="1">binary</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
+  </definedNames>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="21">
   <si>
     <t xml:space="preserve">SELECTING PROFITABLE HOTELS </t>
   </si>
@@ -58,6 +100,30 @@
   </si>
   <si>
     <t>South Lake Tahoe, California</t>
+  </si>
+  <si>
+    <t>Profit</t>
+  </si>
+  <si>
+    <t>Buy/OrNot</t>
+  </si>
+  <si>
+    <t>Objective</t>
+  </si>
+  <si>
+    <t>Constraints</t>
+  </si>
+  <si>
+    <t>&lt;=</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>&lt;-Coefficients</t>
+  </si>
+  <si>
+    <t>Decision Variables</t>
   </si>
 </sst>
 </file>
@@ -65,7 +131,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -84,15 +150,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -186,11 +264,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -213,7 +345,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -222,7 +354,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -236,6 +368,36 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -243,6 +405,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -568,34 +735,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.5" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.125" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="7" width="19.83203125" customWidth="1"/>
+    <col min="6" max="7" width="19.875" customWidth="1"/>
+    <col min="8" max="8" width="12.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" ht="16" thickBot="1">
+      <c r="C1" s="23">
+        <v>39.049999999999997</v>
+      </c>
+      <c r="D1" s="23">
+        <v>5.86</v>
+      </c>
+      <c r="E1" s="23">
+        <v>-3.09</v>
+      </c>
+      <c r="F1" s="23">
+        <v>1.75</v>
+      </c>
+      <c r="G1" s="23">
+        <v>-5.41</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -604,7 +785,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="31" thickBot="1">
+    <row r="3" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -626,8 +807,11 @@
       <c r="G3" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" s="28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -649,8 +833,12 @@
       <c r="G4" s="13">
         <v>-0.99598662130000004</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" s="26">
+        <f>($D$1*D4+$E$1*E4+$F$1*F4+$G$1*G4)+$C$1</f>
+        <v>44.242368789693998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>2</v>
       </c>
@@ -672,8 +860,12 @@
       <c r="G5" s="13">
         <v>-0.47427934350000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5" s="26">
+        <f t="shared" ref="H5:H19" si="0">($D$1*D5+$E$1*E5+$F$1*F5+$G$1*G5)+$C$1</f>
+        <v>53.379192308345999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>3</v>
       </c>
@@ -695,8 +887,12 @@
       <c r="G6" s="13">
         <v>-0.47427934350000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" s="26">
+        <f t="shared" si="0"/>
+        <v>43.021178937635995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>4</v>
       </c>
@@ -718,8 +914,12 @@
       <c r="G7" s="13">
         <v>-0.47427934350000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7" s="26">
+        <f t="shared" si="0"/>
+        <v>42.606858402455998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>5</v>
       </c>
@@ -741,8 +941,12 @@
       <c r="G8" s="13">
         <v>-0.47427934350000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8" s="26">
+        <f t="shared" si="0"/>
+        <v>37.344987610357997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>6</v>
       </c>
@@ -764,8 +968,12 @@
       <c r="G9" s="13">
         <v>-0.55727822859999998</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9" s="26">
+        <f t="shared" si="0"/>
+        <v>49.095069467228996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>7</v>
       </c>
@@ -787,8 +995,12 @@
       <c r="G10" s="13">
         <v>3.1065296996999998</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10" s="26">
+        <f t="shared" si="0"/>
+        <v>23.776865664523996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>8</v>
       </c>
@@ -810,8 +1022,12 @@
       <c r="G11" s="13">
         <v>3.1065296996999998</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11" s="26">
+        <f t="shared" si="0"/>
+        <v>23.445409236965997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>9</v>
       </c>
@@ -833,8 +1049,12 @@
       <c r="G12" s="13">
         <v>3.1065296996999998</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12" s="26">
+        <f t="shared" si="0"/>
+        <v>28.665847975545997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>10</v>
       </c>
@@ -856,8 +1076,12 @@
       <c r="G13" s="13">
         <v>-0.42685140910000002</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="H13" s="26">
+        <f t="shared" si="0"/>
+        <v>38.880673112772996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>11</v>
       </c>
@@ -879,8 +1103,12 @@
       <c r="G14" s="13">
         <v>-0.42685140910000002</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="H14" s="26">
+        <f t="shared" si="0"/>
+        <v>38.010599989480994</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>12</v>
       </c>
@@ -902,8 +1130,12 @@
       <c r="G15" s="13">
         <v>-0.42685140910000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="H15" s="26">
+        <f t="shared" si="0"/>
+        <v>40.289362931212999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>13</v>
       </c>
@@ -925,8 +1157,12 @@
       <c r="G16" s="13">
         <v>-0.42685140910000002</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16" s="26">
+        <f t="shared" si="0"/>
+        <v>39.419289807920997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>14</v>
       </c>
@@ -948,8 +1184,12 @@
       <c r="G17" s="13">
         <v>-0.42685140910000002</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17" s="26">
+        <f t="shared" si="0"/>
+        <v>42.360965605354998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>15</v>
       </c>
@@ -971,8 +1211,12 @@
       <c r="G18" s="13">
         <v>-0.42685140910000002</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="16" thickBot="1">
+      <c r="H18" s="26">
+        <f t="shared" si="0"/>
+        <v>38.590648738146996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <v>16</v>
       </c>
@@ -993,6 +1237,10 @@
       </c>
       <c r="G19" s="15">
         <v>-0.42685140910000002</v>
+      </c>
+      <c r="H19" s="27">
+        <f t="shared" si="0"/>
+        <v>37.389119187296998</v>
       </c>
     </row>
   </sheetData>
@@ -1003,4 +1251,368 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="19.25" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.875" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="18">
+        <v>1</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="20">
+        <v>2925000</v>
+      </c>
+      <c r="E3" s="21">
+        <v>44.242368789693998</v>
+      </c>
+      <c r="F3" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="18">
+        <v>2</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="20">
+        <v>10000000</v>
+      </c>
+      <c r="E4" s="21">
+        <v>53.379192308345999</v>
+      </c>
+      <c r="F4" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="18">
+        <v>3</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="20">
+        <v>3750000</v>
+      </c>
+      <c r="E5" s="21">
+        <v>43.021178937635995</v>
+      </c>
+      <c r="F5" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="18">
+        <v>4</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="20">
+        <v>3500000</v>
+      </c>
+      <c r="E6" s="21">
+        <v>42.606858402455998</v>
+      </c>
+      <c r="F6" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="18">
+        <v>5</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="20">
+        <v>325000</v>
+      </c>
+      <c r="E7" s="21">
+        <v>37.344987610357997</v>
+      </c>
+      <c r="F7" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="18">
+        <v>6</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="20">
+        <v>8950000</v>
+      </c>
+      <c r="E8" s="21">
+        <v>49.095069467228996</v>
+      </c>
+      <c r="F8" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="18">
+        <v>7</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="20">
+        <v>1950000</v>
+      </c>
+      <c r="E9" s="21">
+        <v>23.776865664523996</v>
+      </c>
+      <c r="F9" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="18">
+        <v>8</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="20">
+        <v>1750000</v>
+      </c>
+      <c r="E10" s="21">
+        <v>23.445409236965997</v>
+      </c>
+      <c r="F10" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="18">
+        <v>9</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="20">
+        <v>4900000</v>
+      </c>
+      <c r="E11" s="21">
+        <v>28.665847975545997</v>
+      </c>
+      <c r="F11" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="18">
+        <v>10</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="20">
+        <v>1650000</v>
+      </c>
+      <c r="E12" s="21">
+        <v>38.880673112772996</v>
+      </c>
+      <c r="F12" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="18">
+        <v>11</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="20">
+        <v>1125000</v>
+      </c>
+      <c r="E13" s="21">
+        <v>38.010599989480994</v>
+      </c>
+      <c r="F13" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="18">
+        <v>12</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="20">
+        <v>2500000</v>
+      </c>
+      <c r="E14" s="21">
+        <v>40.289362931212999</v>
+      </c>
+      <c r="F14" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="18">
+        <v>13</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="20">
+        <v>1975000</v>
+      </c>
+      <c r="E15" s="21">
+        <v>39.419289807920997</v>
+      </c>
+      <c r="F15" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="18">
+        <v>14</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="20">
+        <v>3750000</v>
+      </c>
+      <c r="E16" s="21">
+        <v>42.360965605354998</v>
+      </c>
+      <c r="F16" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="18">
+        <v>15</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="20">
+        <v>1475000</v>
+      </c>
+      <c r="E17" s="21">
+        <v>38.590648738146996</v>
+      </c>
+      <c r="F17" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="18">
+        <v>16</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="20">
+        <v>750000</v>
+      </c>
+      <c r="E18" s="21">
+        <v>37.389119187296998</v>
+      </c>
+      <c r="F18" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="25">
+        <f>SUMPRODUCT(E3:E18,F3:F18)</f>
+        <v>205.61804029675994</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="24">
+        <f>SUMPRODUCT(D3:D18,F3:F18)</f>
+        <v>9675000</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="24">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="24">
+        <f>SUM(F12:F18)</f>
+        <v>2</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="24">
+        <f>SUM(F3:F18)</f>
+        <v>6</v>
+      </c>
+      <c r="E24" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="24">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>